<commit_message>
Dashboard updated 6 cases and login page updated - Loginpage and dashboard page
</commit_message>
<xml_diff>
--- a/testdata/Logintutor.xlsx
+++ b/testdata/Logintutor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoges\PycharmProjects\ilrnu\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5452781D-3155-41D1-B17C-DD04E11E5987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC285F3-8010-4662-9085-DF64FA0EEEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,25 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>Testcases</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Login as Tutor with valid username and Password - Postive</t>
-  </si>
-  <si>
-    <t>Login as Tutor with invalid username and Password-Negative</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>yatutor200@gmail.com</t>
   </si>
@@ -47,6 +29,21 @@
   </si>
   <si>
     <t>India@2021</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>loginstatus</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -459,57 +456,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B1C78EDA-262A-4B27-AF25-06758EA3C820}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B1C78EDA-262A-4B27-AF25-06758EA3C820}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>